<commit_message>
email and person preparing sheet is now uploaded
</commit_message>
<xml_diff>
--- a/regolith/templates/coa_template_doe.xlsx
+++ b/regolith/templates/coa_template_doe.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Lead Applicant Organization:</t>
   </si>
@@ -87,15 +87,6 @@
   </si>
   <si>
     <t>advisee</t>
-  </si>
-  <si>
-    <t>Stony Brook University</t>
-  </si>
-  <si>
-    <t>Parise, John</t>
-  </si>
-  <si>
-    <t>John.parise@stonybrook.edu</t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1050,8 @@
   <dimension ref="A1:H411"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G251" sqref="G250:G251"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1079,9 +1070,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="39"/>
-      <c r="C1" s="41" t="s">
-        <v>17</v>
-      </c>
+      <c r="C1" s="41"/>
       <c r="D1" s="41"/>
       <c r="E1" s="2"/>
     </row>
@@ -1090,9 +1079,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="39"/>
-      <c r="C2" s="41" t="s">
-        <v>18</v>
-      </c>
+      <c r="C2" s="41"/>
       <c r="D2" s="41"/>
       <c r="E2" s="2"/>
     </row>
@@ -1101,9 +1088,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="39"/>
-      <c r="C3" s="41" t="s">
-        <v>18</v>
-      </c>
+      <c r="C3" s="41"/>
       <c r="D3" s="41"/>
       <c r="E3" s="2"/>
     </row>
@@ -1112,9 +1097,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="39"/>
-      <c r="C4" s="40" t="s">
-        <v>19</v>
-      </c>
+      <c r="C4" s="40"/>
       <c r="D4" s="41"/>
       <c r="E4" s="2"/>
     </row>
@@ -1126,7 +1109,7 @@
       <c r="B6" s="43"/>
       <c r="C6" s="44" t="str">
         <f>"Collaborator Table - "&amp;C1&amp;" ("&amp;C2&amp;")"</f>
-        <v>Collaborator Table - Stony Brook University (Parise, John)</v>
+        <v>Collaborator Table -  ()</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44"/>
@@ -5365,11 +5348,8 @@
       <formula2>2045</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -5438,21 +5418,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001733C14AC8EC6F498F123411DB8BC020" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1f196d61ef494b6c4f62f58be5bb14e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7b7cc8fe-90e2-43f3-ad3c-00f457ec8258" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46c76a5a58717c3453de3c52cd271f55" ns2:_="">
     <xsd:import namespace="7b7cc8fe-90e2-43f3-ad3c-00f457ec8258"/>
@@ -5584,31 +5549,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ACD002-FFBE-4185-9DDB-0AA3A824C3C1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ACA6411-41A0-4B6C-874D-1FC05CC4B568}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7b7cc8fe-90e2-43f3-ad3c-00f457ec8258"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE70D9AC-1270-4AD5-BB63-23D2B0A32B51}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5624,4 +5580,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7ACA6411-41A0-4B6C-874D-1FC05CC4B568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7b7cc8fe-90e2-43f3-ad3c-00f457ec8258"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ACD002-FFBE-4185-9DDB-0AA3A824C3C1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>